<commit_message>
chore: clean up data
</commit_message>
<xml_diff>
--- a/Final_Student_Grade_Report.xlsx
+++ b/Final_Student_Grade_Report.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,7 +963,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Last year of college</t>
+          <t>Final year of college</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>First Year</t>
+          <t>College</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>First year of college</t>
+          <t>1st year of college</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Year 1 of College</t>
+          <t>1st year of college</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Second year of college</t>
+          <t>2nd year of college</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1465,12 +1465,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Midkent college</t>
+          <t>Midkent College</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Business level 3 first year</t>
+          <t>2nd year of college</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1499,17 +1499,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Shalom Dube</t>
+          <t>Shalom Mutongi</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Midkent College</t>
+          <t>Midkent college</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Business level 3  final yeah</t>
+          <t>Year 12</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1538,34 +1538,34 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Shalom Mutongi</t>
+          <t>Sharlom Verengera</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Midkent college</t>
+          <t>Holcombe Grammar</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Year 12</t>
+          <t>Year 13</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
         <v>1</v>
       </c>
-      <c r="G29" t="n">
-        <v>0</v>
-      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1577,12 +1577,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sharlom Verengera</t>
+          <t>Soala Frank-Briggs</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Holcombe Grammar</t>
+          <t>Invicta Grammar School</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1594,17 +1594,17 @@
         <v>3</v>
       </c>
       <c r="E30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1616,73 +1616,73 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Soala Frank-Briggs</t>
+          <t>Sophia Nnabue</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Invicta Grammar School</t>
+          <t>Rochester Grammar School for Girls</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Year 13</t>
+          <t>Year 10</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Sophia Nnabue</t>
+          <t>Toluwanimi Asaju</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Rochester Grammar School for Girls</t>
+          <t>Chatham Grammar</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Year 10</t>
+          <t>Year 13</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -1694,21 +1694,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Toluwanimi Asaju</t>
+          <t>Victoria Adebayo</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Chatham Grammar</t>
+          <t>Midkent college</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Year 13</t>
+          <t>2nd year of college</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1717,92 +1717,53 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Victoria Adebayo</t>
+          <t>Victoria Dina</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Midkent college</t>
+          <t>Fort pitt grammar school</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lv 3 yr2 / yr 13</t>
+          <t>Year 12</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Victoria Dina</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Fort pitt grammar school</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Year 12</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1819,7 +1780,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4150,7 +4111,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Last year of college</t>
+          <t>Final year of college</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -5830,7 +5791,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>First Year</t>
+          <t>College</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -5872,7 +5833,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>First year of college</t>
+          <t>1st year of college</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -6040,7 +6001,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Year 1 of College</t>
+          <t>1st year of college</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -6082,7 +6043,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Year 1 of College</t>
+          <t>1st year of college</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -6376,7 +6337,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Second year of college</t>
+          <t>2nd year of college</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -6413,12 +6374,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Midkent college</t>
+          <t>Midkent College</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Business level 3 first year</t>
+          <t>2nd year of college</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -6450,17 +6411,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Shalom Dube</t>
+          <t>Shalom Mutongi</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Midkent College</t>
+          <t>Midkent college</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Business level 3  final yeah</t>
+          <t>Year 12</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -6470,17 +6431,17 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Distinction</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Distinction</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Meeting Target</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -6492,42 +6453,42 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Shalom Mutongi</t>
+          <t>Sharlom Verengera</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Midkent college</t>
+          <t>Holcombe Grammar</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Year 12</t>
+          <t>Year 13</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Business Studies</t>
+          <t>Religious Studies</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Distinction</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Distinction</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Meeting Target</t>
+          <t>Below Target</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -6549,7 +6510,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Religious Studies</t>
+          <t>English Literature</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -6559,12 +6520,12 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Below Target</t>
+          <t>Meeting Target</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -6591,7 +6552,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>English Literature</t>
+          <t>Psychology</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -6618,12 +6579,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Sharlom Verengera</t>
+          <t>Soala Frank-Briggs</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Holcombe Grammar</t>
+          <t>Invicta Grammar School</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -6633,17 +6594,17 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Psychology</t>
+          <t>English Literature</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -6653,7 +6614,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -6675,22 +6636,22 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>English Literature</t>
+          <t>History</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Meeting Target</t>
+          <t>Exceeding Target</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -6717,7 +6678,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>History</t>
+          <t>Business Studies</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -6744,42 +6705,42 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Soala Frank-Briggs</t>
+          <t>Sophia Nnabue</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Invicta Grammar School</t>
+          <t>Rochester Grammar School for Girls</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Year 13</t>
+          <t>Year 10</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Business Studies</t>
+          <t>Biology</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Exceeding Target</t>
+          <t>Meeting Target</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
     </row>
@@ -6801,7 +6762,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -6843,22 +6804,22 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Physics</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Meeting Target</t>
+          <t>Below Target</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -6885,12 +6846,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>Mathematics</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -6927,12 +6888,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>English Language</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -6969,7 +6930,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>English Language</t>
+          <t>English Literature</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -7011,22 +6972,22 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>English Literature</t>
+          <t>Sociology</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Below Target</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -7053,22 +7014,22 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Sociology</t>
+          <t>History</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Meeting Target</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -7095,7 +7056,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>History</t>
+          <t>Music</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -7137,7 +7098,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Religious Studies</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -7164,42 +7125,42 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Sophia Nnabue</t>
+          <t>Toluwanimi Asaju</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Rochester Grammar School for Girls</t>
+          <t>Chatham Grammar</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Year 10</t>
+          <t>Year 13</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Religious Studies</t>
+          <t>Economics</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Meeting Target</t>
+          <t>Below Target</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -7221,12 +7182,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Economics</t>
+          <t>Business Studies</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -7248,17 +7209,17 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Toluwanimi Asaju</t>
+          <t>Victoria Adebayo</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Chatham Grammar</t>
+          <t>Midkent college</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Year 13</t>
+          <t>2nd year of college</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -7268,64 +7229,64 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Below Target</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Victoria Adebayo</t>
+          <t>Victoria Dina</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Midkent college</t>
+          <t>Fort pitt grammar school</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Lv 3 yr2 / yr 13</t>
+          <t>Year 12</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Business Studies</t>
+          <t>Mathematics</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A*</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>Below Target</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -7347,12 +7308,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Biology</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>A*</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -7362,7 +7323,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Below Target</t>
+          <t>Meeting Target</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -7389,7 +7350,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -7431,67 +7392,25 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Psychology</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
           <t>A*</t>
         </is>
       </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>A*</t>
-        </is>
-      </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Meeting Target</t>
+          <t>Target Set</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>Victoria Dina</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Fort pitt grammar school</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Year 12</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>Psychology</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>A*</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>Target Set</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>

</xml_diff>